<commit_message>
updated for arduino elevator control
</commit_message>
<xml_diff>
--- a/electrical/astrowiring_diagram.xlsx
+++ b/electrical/astrowiring_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\School\2018-19\Spring\ECE 4990-001        IEEE Robotics\astrohub\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1018EE02-7A2F-49DB-BC61-96BE24EDA862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2C991B-D44E-4BCA-A0F8-70896BB53BD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="143">
   <si>
     <t>Raspberry Pi 3B</t>
   </si>
@@ -430,6 +430,30 @@
   </si>
   <si>
     <t>*splice wire into two</t>
+  </si>
+  <si>
+    <t>Stepper</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>ENABLE</t>
+  </si>
+  <si>
+    <t>BREAK</t>
   </si>
 </sst>
 </file>
@@ -600,7 +624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -635,17 +659,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -655,30 +668,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -726,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -741,40 +734,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -893,19 +868,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -935,6 +910,78 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>182217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8282</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DDD7D8-FD6E-442D-8EF5-A82B21FF371F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5449957" y="1896717"/>
+          <a:ext cx="3097695" cy="1358348"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1200,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,30 +1260,31 @@
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="61"/>
-      <c r="K2" s="62"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
       <c r="L2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="59"/>
+      <c r="E3" s="54"/>
       <c r="I3" s="3" t="s">
         <v>78</v>
       </c>
@@ -1252,7 +1300,7 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="37">
         <v>1</v>
       </c>
       <c r="E4" s="1">
@@ -1262,7 +1310,7 @@
         <v>26</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="21" t="s">
         <v>70</v>
       </c>
       <c r="J4" s="2">
@@ -1279,7 +1327,7 @@
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="31">
         <v>3</v>
       </c>
       <c r="E5" s="1">
@@ -1289,7 +1337,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="14" t="s">
         <v>71</v>
       </c>
       <c r="J5" s="2">
@@ -1306,7 +1354,7 @@
       <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="32">
         <v>5</v>
       </c>
       <c r="E6" s="1">
@@ -1316,7 +1364,7 @@
         <v>101</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="13" t="s">
         <v>72</v>
       </c>
       <c r="J6" s="2">
@@ -1333,10 +1381,10 @@
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="38">
         <v>7</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="12">
         <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1345,7 +1393,7 @@
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="20" t="s">
         <v>73</v>
       </c>
       <c r="J7" s="2">
@@ -1372,7 +1420,7 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="15" t="s">
         <v>74</v>
       </c>
       <c r="J8" s="2">
@@ -1401,7 +1449,7 @@
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="17" t="s">
         <v>116</v>
       </c>
       <c r="J9" s="2">
@@ -1418,7 +1466,7 @@
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="42">
         <v>13</v>
       </c>
       <c r="E10" s="1">
@@ -1436,7 +1484,7 @@
       <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="43">
         <v>15</v>
       </c>
       <c r="E11" s="1">
@@ -1448,18 +1496,18 @@
       <c r="G11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="44">
         <v>17</v>
       </c>
       <c r="E12" s="1">
@@ -1488,7 +1536,7 @@
       <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="17">
         <v>19</v>
       </c>
       <c r="E13" s="1">
@@ -1498,7 +1546,7 @@
         <v>101</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="16" t="s">
         <v>76</v>
       </c>
       <c r="J13" s="2">
@@ -1515,10 +1563,10 @@
       <c r="C14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="10">
         <v>21</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="1">
         <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1527,7 +1575,7 @@
       <c r="G14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="17" t="s">
         <v>79</v>
       </c>
       <c r="J14" s="2">
@@ -1544,10 +1592,10 @@
       <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>23</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="1">
         <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1556,7 +1604,7 @@
       <c r="G15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="23" t="s">
         <v>80</v>
       </c>
       <c r="J15" s="2">
@@ -1574,7 +1622,7 @@
       <c r="D16" s="6">
         <v>25</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="1">
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1583,7 +1631,7 @@
       <c r="G16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="18" t="s">
         <v>81</v>
       </c>
       <c r="J16" s="2">
@@ -1600,10 +1648,10 @@
       <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="8">
         <v>27</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="1">
         <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1612,7 +1660,7 @@
       <c r="G17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="19" t="s">
         <v>82</v>
       </c>
       <c r="J17" s="2">
@@ -1629,10 +1677,10 @@
       <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="11">
         <v>29</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="1">
         <v>30</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1647,10 +1695,10 @@
       <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="9">
         <v>31</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="1">
         <v>32</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1659,19 +1707,19 @@
       <c r="G19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="L19" s="35" t="s">
+      <c r="L19" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="M19" s="35" t="s">
+      <c r="M19" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="N19" s="35" t="s">
+      <c r="N19" s="29" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1692,19 +1740,19 @@
         <v>101</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="22">
         <v>3</v>
       </c>
-      <c r="L20" s="45" t="s">
+      <c r="L20" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20" s="22">
         <v>17</v>
       </c>
-      <c r="N20" s="28"/>
+      <c r="N20" s="22"/>
       <c r="O20" t="s">
         <v>134</v>
       </c>
@@ -1728,19 +1776,19 @@
       <c r="G21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="22">
         <v>5</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="M21" s="28">
+      <c r="M21" s="22">
         <v>13</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="22">
         <v>2</v>
       </c>
     </row>
@@ -1760,13 +1808,13 @@
       <c r="G22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L22" s="47" t="s">
+      <c r="L22" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="28">
+      <c r="M22" s="22">
         <v>14</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N22" s="22">
         <v>0</v>
       </c>
     </row>
@@ -1787,51 +1835,51 @@
       <c r="G23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="J23" s="35" t="s">
+      <c r="J23" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K23" s="29" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="63"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="22">
         <v>1</v>
       </c>
-      <c r="K24" s="28"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="I25" s="42" t="s">
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="I25" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="22">
         <v>7</v>
       </c>
-      <c r="K25" s="28">
+      <c r="K25" s="22">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="59"/>
+      <c r="E26" s="54"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
@@ -1903,40 +1951,52 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="s">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="D35" s="59" t="s">
+    <row r="35" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D35" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="59"/>
-      <c r="H35" s="35" t="s">
+      <c r="E35" s="54"/>
+      <c r="H35" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I35" s="35" t="s">
+      <c r="I35" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="K35" s="33" t="s">
+      <c r="K35" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="L35" s="33" t="s">
+      <c r="L35" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="M35" s="33" t="s">
+      <c r="M35" s="27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O35" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="P35" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="R35" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="S35" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="D36" s="5" t="s">
         <v>85</v>
@@ -1944,23 +2004,35 @@
       <c r="E36" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H36" s="40" t="s">
+      <c r="H36" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="I36" s="28" t="s">
+      <c r="I36" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="K36" s="64">
+      <c r="K36" s="58">
         <v>1</v>
       </c>
-      <c r="L36" s="58" t="s">
+      <c r="L36" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="M36" s="39" t="s">
+      <c r="M36" s="33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O36" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="P36" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="R36" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="S36" s="33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="D37" s="5" t="s">
         <v>86</v>
@@ -1968,21 +2040,27 @@
       <c r="E37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H37" s="57" t="s">
+      <c r="H37" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="I37" s="28" t="s">
+      <c r="I37" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="K37" s="64"/>
-      <c r="L37" s="34" t="s">
+      <c r="K37" s="58"/>
+      <c r="L37" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="M37" s="39" t="s">
+      <c r="M37" s="33" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O37" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="P37" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="D38" s="5" t="s">
         <v>87</v>
@@ -1990,23 +2068,29 @@
       <c r="E38" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H38" s="52" t="s">
+      <c r="H38" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="I38" s="28" t="s">
+      <c r="I38" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="K38" s="64">
+      <c r="K38" s="58">
         <v>2</v>
       </c>
-      <c r="L38" s="53" t="s">
+      <c r="L38" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="M38" s="39" t="s">
+      <c r="M38" s="33" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O38" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="P38" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="D39" s="5" t="s">
         <v>101</v>
@@ -2014,121 +2098,139 @@
       <c r="E39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="51" t="s">
+      <c r="H39" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="I39" s="28" t="s">
+      <c r="I39" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="K39" s="64"/>
-      <c r="L39" s="55" t="s">
+      <c r="K39" s="58"/>
+      <c r="L39" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="M39" s="39" t="s">
+      <c r="M39" s="33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="31"/>
-      <c r="D40" s="58" t="s">
+      <c r="O39" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="P39" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="25"/>
+      <c r="D40" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="K40" s="64">
+      <c r="K40" s="58">
         <v>3</v>
       </c>
-      <c r="L40" s="54" t="s">
+      <c r="L40" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="M40" s="39" t="s">
+      <c r="M40" s="33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O40" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="P40" s="33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="51" t="s">
+      <c r="D41" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="K41" s="64"/>
-      <c r="L41" s="56" t="s">
+      <c r="K41" s="58"/>
+      <c r="L41" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="M41" s="39" t="s">
+      <c r="M41" s="33" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O41" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="P41" s="33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C42" s="5"/>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="53" t="s">
+      <c r="D43" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="28" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="55" t="s">
+      <c r="D44" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="47" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C45" s="5"/>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="49" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C46" s="5"/>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="40" t="s">
+      <c r="D47" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="50" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="57" t="s">
+      <c r="D48" s="51" t="s">
         <v>96</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -2139,7 +2241,7 @@
       <c r="C49" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="46" t="s">
         <v>97</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -2156,14 +2258,14 @@
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="63" t="s">
+      <c r="D51" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="E51" s="63"/>
+      <c r="E51" s="53"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D53" s="5"/>
@@ -2179,20 +2281,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D24:E25"/>
     <mergeCell ref="D51:E52"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="K36:K37"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="K40:K41"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D24:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>